<commit_message>
Se corrige error en importancion de excel
</commit_message>
<xml_diff>
--- a/admin/upload/generales/cop_listamateriales.xlsx
+++ b/admin/upload/generales/cop_listamateriales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cert\sistema\siaa\admin\ajax-save\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18002A11-0E7C-4EA8-A6A1-C4A8BC0543FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18A3EAA-4234-4BA3-8CFE-880F724664AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC19406E-DE80-4DCF-B2A3-5A470C991D95}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>nombre</t>
   </si>
@@ -41,79 +41,10 @@
     <t>descripcion</t>
   </si>
   <si>
-    <t>prueba 1</t>
-  </si>
-  <si>
-    <t>prueba 2</t>
-  </si>
-  <si>
-    <t>prueba 3</t>
-  </si>
-  <si>
-    <t>prueba 4</t>
-  </si>
-  <si>
-    <t>prueba 5</t>
-  </si>
-  <si>
-    <t>prueba 6</t>
-  </si>
-  <si>
-    <t>prueba 7</t>
-  </si>
-  <si>
-    <t>prueba 8</t>
-  </si>
-  <si>
-    <t>prueba 9</t>
-  </si>
-  <si>
-    <t>prueba 10</t>
-  </si>
-  <si>
-    <t>prueba 11</t>
-  </si>
-  <si>
-    <t>prueba 12</t>
-  </si>
-  <si>
-    <t>prueba 13</t>
-  </si>
-  <si>
-    <t>prueba 14</t>
-  </si>
-  <si>
-    <t>prueba 15</t>
-  </si>
-  <si>
-    <t>prueba 16</t>
-  </si>
-  <si>
-    <t>prueba 17</t>
-  </si>
-  <si>
-    <t>prueba 18</t>
-  </si>
-  <si>
     <t>numero_serie</t>
   </si>
   <si>
     <t>unidad</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>GAL</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
 </sst>
 </file>
@@ -471,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B17104E-0A96-4DFE-BA76-7B7726536C20}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,262 +421,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1651</v>
-      </c>
-      <c r="C2">
-        <v>3206</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1652</v>
-      </c>
-      <c r="C3">
-        <v>3207</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1653</v>
-      </c>
-      <c r="C4">
-        <v>3208</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1654</v>
-      </c>
-      <c r="C5">
-        <v>3209</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>1655</v>
-      </c>
-      <c r="C6">
-        <v>3210</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>1656</v>
-      </c>
-      <c r="C7">
-        <v>3211</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>1657</v>
-      </c>
-      <c r="C8">
-        <v>3212</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>1658</v>
-      </c>
-      <c r="C9">
-        <v>3213</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>1659</v>
-      </c>
-      <c r="C10">
-        <v>3214</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>1660</v>
-      </c>
-      <c r="C11">
-        <v>3215</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>1661</v>
-      </c>
-      <c r="C12">
-        <v>3216</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>1662</v>
-      </c>
-      <c r="C13">
-        <v>3217</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>1663</v>
-      </c>
-      <c r="C14">
-        <v>3218</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>1664</v>
-      </c>
-      <c r="C15">
-        <v>3219</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>1665</v>
-      </c>
-      <c r="C16">
-        <v>3220</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>1666</v>
-      </c>
-      <c r="C17">
-        <v>3221</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>1667</v>
-      </c>
-      <c r="C18">
-        <v>3222</v>
-      </c>
-      <c r="D18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>1668</v>
-      </c>
-      <c r="C19">
-        <v>3223</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>